<commit_message>
Update lexical diversity to count as proportion of all tokens, not just word tokens
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/news_and_blog/Fakespeak_news_and_blog_lexical_diversity.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/news_and_blog/Fakespeak_news_and_blog_lexical_diversity.xlsx
@@ -1851,7 +1851,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>0.796875</v>
+        <v>0.7567567567567568</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1859,7 +1859,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>0.5233918128654971</v>
+        <v>0.4594594594594595</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1867,7 +1867,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>0.5194805194805194</v>
+        <v>0.4507299270072992</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1875,7 +1875,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>0.6150234741784038</v>
+        <v>0.5785123966942148</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -1883,7 +1883,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.46875</v>
+        <v>0.4327868852459016</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -1891,7 +1891,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>0.4293865905848788</v>
+        <v>0.3843283582089552</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -1899,7 +1899,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>0.5144694533762058</v>
+        <v>0.4744318181818182</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1907,7 +1907,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>0.5615615615615616</v>
+        <v>0.5131578947368421</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1915,7 +1915,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>0.5903614457831325</v>
+        <v>0.5441696113074205</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1923,7 +1923,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>0.3518072289156626</v>
+        <v>0.3138493944181148</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -1931,7 +1931,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>0.3421400264200792</v>
+        <v>0.316588785046729</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -1939,7 +1939,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>0.4866785079928952</v>
+        <v>0.4238805970149254</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -1947,7 +1947,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>0.3936269915651359</v>
+        <v>0.3516572352465643</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1955,7 +1955,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>0.5366726296958855</v>
+        <v>0.4983974358974359</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1963,7 +1963,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>0.4614147909967846</v>
+        <v>0.415666901905434</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1971,7 +1971,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>0.3451053283767038</v>
+        <v>0.2982273201251304</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -1979,7 +1979,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>0.5718954248366013</v>
+        <v>0.5124653739612188</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1987,7 +1987,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>0.5904059040590406</v>
+        <v>0.5294117647058824</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -1995,7 +1995,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>0.7671232876712328</v>
+        <v>0.7317073170731707</v>
       </c>
     </row>
   </sheetData>
@@ -2024,7 +2024,7 @@
         <v>21</v>
       </c>
       <c r="B2">
-        <v>0.5761904761904761</v>
+        <v>0.516260162601626</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2032,7 +2032,7 @@
         <v>22</v>
       </c>
       <c r="B3">
-        <v>0.4944444444444445</v>
+        <v>0.4467741935483871</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2040,7 +2040,7 @@
         <v>23</v>
       </c>
       <c r="B4">
-        <v>0.3748796920115496</v>
+        <v>0.3235533822330888</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2048,7 +2048,7 @@
         <v>24</v>
       </c>
       <c r="B5">
-        <v>0.8857142857142857</v>
+        <v>0.868421052631579</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2056,7 +2056,7 @@
         <v>25</v>
       </c>
       <c r="B6">
-        <v>0.5297029702970297</v>
+        <v>0.46723044397463</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2064,7 +2064,7 @@
         <v>26</v>
       </c>
       <c r="B7">
-        <v>0.3037747153984422</v>
+        <v>0.2516347783967062</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2072,7 +2072,7 @@
         <v>27</v>
       </c>
       <c r="B8">
-        <v>0.3373493975903614</v>
+        <v>0.2967252396166134</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2080,7 +2080,7 @@
         <v>28</v>
       </c>
       <c r="B9">
-        <v>0.4501160092807425</v>
+        <v>0.4182194616977226</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2088,7 +2088,7 @@
         <v>29</v>
       </c>
       <c r="B10">
-        <v>0.6378600823045267</v>
+        <v>0.5673758865248227</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2096,7 +2096,7 @@
         <v>30</v>
       </c>
       <c r="B11">
-        <v>0.5382716049382716</v>
+        <v>0.4789915966386555</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2104,7 +2104,7 @@
         <v>31</v>
       </c>
       <c r="B12">
-        <v>0.4779050736497545</v>
+        <v>0.4346590909090909</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2112,7 +2112,7 @@
         <v>32</v>
       </c>
       <c r="B13">
-        <v>0.6515151515151515</v>
+        <v>0.5732484076433121</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -2120,7 +2120,7 @@
         <v>33</v>
       </c>
       <c r="B14">
-        <v>0.5369649805447471</v>
+        <v>0.4786885245901639</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -2128,7 +2128,7 @@
         <v>34</v>
       </c>
       <c r="B15">
-        <v>0.4265536723163842</v>
+        <v>0.3777239709443099</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -2136,7 +2136,7 @@
         <v>35</v>
       </c>
       <c r="B16">
-        <v>0.3522041763341067</v>
+        <v>0.309674861221253</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -2144,7 +2144,7 @@
         <v>36</v>
       </c>
       <c r="B17">
-        <v>0.6055776892430279</v>
+        <v>0.5614035087719298</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -2152,7 +2152,7 @@
         <v>37</v>
       </c>
       <c r="B18">
-        <v>0.618421052631579</v>
+        <v>0.5536723163841808</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -2160,7 +2160,7 @@
         <v>38</v>
       </c>
       <c r="B19">
-        <v>0.5278592375366569</v>
+        <v>0.4921465968586388</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -2168,7 +2168,7 @@
         <v>39</v>
       </c>
       <c r="B20">
-        <v>0.3605683836589698</v>
+        <v>0.3100890207715133</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -2176,7 +2176,7 @@
         <v>40</v>
       </c>
       <c r="B21">
-        <v>0.5205479452054794</v>
+        <v>0.4712990936555891</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -2184,7 +2184,7 @@
         <v>41</v>
       </c>
       <c r="B22">
-        <v>0.6289308176100629</v>
+        <v>0.572972972972973</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -2192,7 +2192,7 @@
         <v>42</v>
       </c>
       <c r="B23">
-        <v>0.5307443365695793</v>
+        <v>0.4648648648648649</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -2200,7 +2200,7 @@
         <v>43</v>
       </c>
       <c r="B24">
-        <v>0.6853932584269663</v>
+        <v>0.6018518518518519</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -2208,7 +2208,7 @@
         <v>44</v>
       </c>
       <c r="B25">
-        <v>0.6021505376344086</v>
+        <v>0.5161290322580645</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -2216,7 +2216,7 @@
         <v>45</v>
       </c>
       <c r="B26">
-        <v>0.5461741424802111</v>
+        <v>0.4700854700854701</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -2224,7 +2224,7 @@
         <v>46</v>
       </c>
       <c r="B27">
-        <v>0.5601659751037344</v>
+        <v>0.4805414551607445</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -2232,7 +2232,7 @@
         <v>47</v>
       </c>
       <c r="B28">
-        <v>0.6821192052980133</v>
+        <v>0.5958549222797928</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -2240,7 +2240,7 @@
         <v>48</v>
       </c>
       <c r="B29">
-        <v>0.59375</v>
+        <v>0.5390625</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -2248,7 +2248,7 @@
         <v>49</v>
       </c>
       <c r="B30">
-        <v>0.392548596112311</v>
+        <v>0.360408560311284</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -2256,7 +2256,7 @@
         <v>50</v>
       </c>
       <c r="B31">
-        <v>0.446078431372549</v>
+        <v>0.3938973647711512</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -2264,7 +2264,7 @@
         <v>51</v>
       </c>
       <c r="B32">
-        <v>0.3704716336295283</v>
+        <v>0.3228438228438228</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -2272,7 +2272,7 @@
         <v>52</v>
       </c>
       <c r="B33">
-        <v>0.4259634888438134</v>
+        <v>0.3794871794871795</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -2280,7 +2280,7 @@
         <v>53</v>
       </c>
       <c r="B34">
-        <v>0.4807692307692308</v>
+        <v>0.4422604422604423</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -2288,7 +2288,7 @@
         <v>54</v>
       </c>
       <c r="B35">
-        <v>0.5367847411444142</v>
+        <v>0.4895591647331787</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -2296,7 +2296,7 @@
         <v>55</v>
       </c>
       <c r="B36">
-        <v>0.4603580562659846</v>
+        <v>0.4048140043763676</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -2304,7 +2304,7 @@
         <v>56</v>
       </c>
       <c r="B37">
-        <v>0.6225490196078431</v>
+        <v>0.5879828326180258</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -2312,7 +2312,7 @@
         <v>57</v>
       </c>
       <c r="B38">
-        <v>0.6581632653061225</v>
+        <v>0.5748987854251012</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -2320,7 +2320,7 @@
         <v>58</v>
       </c>
       <c r="B39">
-        <v>0.4318766066838046</v>
+        <v>0.3876651982378855</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -2328,7 +2328,7 @@
         <v>59</v>
       </c>
       <c r="B40">
-        <v>0.3744588744588744</v>
+        <v>0.3409306742640076</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -2336,7 +2336,7 @@
         <v>60</v>
       </c>
       <c r="B41">
-        <v>0.6024844720496895</v>
+        <v>0.546875</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -2344,7 +2344,7 @@
         <v>61</v>
       </c>
       <c r="B42">
-        <v>0.4189315838800375</v>
+        <v>0.3690095846645368</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -2352,7 +2352,7 @@
         <v>62</v>
       </c>
       <c r="B43">
-        <v>0.297877914592612</v>
+        <v>0.264584290307763</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -2360,7 +2360,7 @@
         <v>63</v>
       </c>
       <c r="B44">
-        <v>0.4786053882725832</v>
+        <v>0.4333800841514727</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -2368,7 +2368,7 @@
         <v>64</v>
       </c>
       <c r="B45">
-        <v>0.521311475409836</v>
+        <v>0.4702549575070821</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -2376,7 +2376,7 @@
         <v>65</v>
       </c>
       <c r="B46">
-        <v>0.4509803921568628</v>
+        <v>0.4052132701421801</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -2384,7 +2384,7 @@
         <v>66</v>
       </c>
       <c r="B47">
-        <v>0.4877049180327869</v>
+        <v>0.4411247803163444</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -2392,7 +2392,7 @@
         <v>67</v>
       </c>
       <c r="B48">
-        <v>0.543026706231454</v>
+        <v>0.4798994974874372</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -2400,7 +2400,7 @@
         <v>68</v>
       </c>
       <c r="B49">
-        <v>0.4233128834355828</v>
+        <v>0.3804537521815008</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -2408,7 +2408,7 @@
         <v>69</v>
       </c>
       <c r="B50">
-        <v>0.4160583941605839</v>
+        <v>0.3601953601953602</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -2416,7 +2416,7 @@
         <v>70</v>
       </c>
       <c r="B51">
-        <v>0.3881230116648993</v>
+        <v>0.3519553072625698</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -2424,7 +2424,7 @@
         <v>71</v>
       </c>
       <c r="B52">
-        <v>0.3897180762852405</v>
+        <v>0.3393103448275862</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -2432,7 +2432,7 @@
         <v>72</v>
       </c>
       <c r="B53">
-        <v>0.6691176470588235</v>
+        <v>0.5963855421686747</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -2440,7 +2440,7 @@
         <v>73</v>
       </c>
       <c r="B54">
-        <v>0.6305732484076433</v>
+        <v>0.5765027322404371</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -2448,7 +2448,7 @@
         <v>74</v>
       </c>
       <c r="B55">
-        <v>0.6415094339622641</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -2456,7 +2456,7 @@
         <v>75</v>
       </c>
       <c r="B56">
-        <v>0.6111111111111112</v>
+        <v>0.5697674418604651</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -2464,7 +2464,7 @@
         <v>76</v>
       </c>
       <c r="B57">
-        <v>0.5787545787545788</v>
+        <v>0.5359477124183006</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -2472,7 +2472,7 @@
         <v>77</v>
       </c>
       <c r="B58">
-        <v>0.95</v>
+        <v>0.9565217391304348</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -2480,7 +2480,7 @@
         <v>78</v>
       </c>
       <c r="B59">
-        <v>0.460431654676259</v>
+        <v>0.4184100418410042</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -2488,7 +2488,7 @@
         <v>79</v>
       </c>
       <c r="B60">
-        <v>0.4522388059701493</v>
+        <v>0.4046094750320102</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -2496,7 +2496,7 @@
         <v>80</v>
       </c>
       <c r="B61">
-        <v>0.3446553446553446</v>
+        <v>0.2972292191435768</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -2504,7 +2504,7 @@
         <v>81</v>
       </c>
       <c r="B62">
-        <v>0.4843982169390788</v>
+        <v>0.4276729559748428</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -2512,7 +2512,7 @@
         <v>82</v>
       </c>
       <c r="B63">
-        <v>0.3772819472616633</v>
+        <v>0.3413547237076649</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -2520,7 +2520,7 @@
         <v>83</v>
       </c>
       <c r="B64">
-        <v>0.4893162393162393</v>
+        <v>0.4555765595463138</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -2528,7 +2528,7 @@
         <v>84</v>
       </c>
       <c r="B65">
-        <v>0.3891547049441786</v>
+        <v>0.3543956043956044</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -2536,7 +2536,7 @@
         <v>85</v>
       </c>
       <c r="B66">
-        <v>0.5573770491803278</v>
+        <v>0.4891891891891892</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -2544,7 +2544,7 @@
         <v>86</v>
       </c>
       <c r="B67">
-        <v>0.4642857142857143</v>
+        <v>0.405320813771518</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -2552,7 +2552,7 @@
         <v>87</v>
       </c>
       <c r="B68">
-        <v>0.4769736842105263</v>
+        <v>0.428169014084507</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -2560,7 +2560,7 @@
         <v>88</v>
       </c>
       <c r="B69">
-        <v>0.4483925549915397</v>
+        <v>0.4038461538461539</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -2568,7 +2568,7 @@
         <v>89</v>
       </c>
       <c r="B70">
-        <v>0.4610526315789474</v>
+        <v>0.4237918215613383</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -2576,7 +2576,7 @@
         <v>90</v>
       </c>
       <c r="B71">
-        <v>0.4447086801426873</v>
+        <v>0.39648033126294</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -2584,7 +2584,7 @@
         <v>91</v>
       </c>
       <c r="B72">
-        <v>0.3736713000817661</v>
+        <v>0.3165322580645161</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -2592,7 +2592,7 @@
         <v>92</v>
       </c>
       <c r="B73">
-        <v>0.4553119730185498</v>
+        <v>0.4195488721804511</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -2600,7 +2600,7 @@
         <v>93</v>
       </c>
       <c r="B74">
-        <v>0.4153132250580047</v>
+        <v>0.355899419729207</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -2608,7 +2608,7 @@
         <v>94</v>
       </c>
       <c r="B75">
-        <v>0.5524296675191815</v>
+        <v>0.4732334047109208</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -2616,7 +2616,7 @@
         <v>95</v>
       </c>
       <c r="B76">
-        <v>0.5708661417322834</v>
+        <v>0.4841772151898734</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -2624,7 +2624,7 @@
         <v>96</v>
       </c>
       <c r="B77">
-        <v>0.4317617866004963</v>
+        <v>0.3767820773930753</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -2632,7 +2632,7 @@
         <v>97</v>
       </c>
       <c r="B78">
-        <v>0.5283842794759825</v>
+        <v>0.4650735294117647</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -2640,7 +2640,7 @@
         <v>98</v>
       </c>
       <c r="B79">
-        <v>0.4666666666666667</v>
+        <v>0.4247311827956989</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -2648,7 +2648,7 @@
         <v>99</v>
       </c>
       <c r="B80">
-        <v>0.5118790496760259</v>
+        <v>0.4414414414414414</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -2656,7 +2656,7 @@
         <v>100</v>
       </c>
       <c r="B81">
-        <v>0.5009940357852882</v>
+        <v>0.440536013400335</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -2664,7 +2664,7 @@
         <v>101</v>
       </c>
       <c r="B82">
-        <v>0.4274028629856851</v>
+        <v>0.3859964093357271</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -2672,7 +2672,7 @@
         <v>102</v>
       </c>
       <c r="B83">
-        <v>0.5643044619422573</v>
+        <v>0.5150115473441108</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -2680,7 +2680,7 @@
         <v>103</v>
       </c>
       <c r="B84">
-        <v>0.7341772151898734</v>
+        <v>0.6595744680851063</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -2688,7 +2688,7 @@
         <v>104</v>
       </c>
       <c r="B85">
-        <v>0.7142857142857143</v>
+        <v>0.6585365853658537</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -2696,7 +2696,7 @@
         <v>105</v>
       </c>
       <c r="B86">
-        <v>0.5165289256198347</v>
+        <v>0.4784172661870504</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -2704,7 +2704,7 @@
         <v>106</v>
       </c>
       <c r="B87">
-        <v>0.6448598130841121</v>
+        <v>0.5826771653543307</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -2712,7 +2712,7 @@
         <v>107</v>
       </c>
       <c r="B88">
-        <v>0.6496350364963503</v>
+        <v>0.6089743589743589</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -2720,7 +2720,7 @@
         <v>108</v>
       </c>
       <c r="B89">
-        <v>0.5626911314984709</v>
+        <v>0.5188172043010753</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -2728,7 +2728,7 @@
         <v>109</v>
       </c>
       <c r="B90">
-        <v>0.5140324963072378</v>
+        <v>0.4481897627965044</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -2736,7 +2736,7 @@
         <v>110</v>
       </c>
       <c r="B91">
-        <v>0.5454545454545454</v>
+        <v>0.5238095238095238</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -2744,7 +2744,7 @@
         <v>111</v>
       </c>
       <c r="B92">
-        <v>0.5533333333333333</v>
+        <v>0.5181818181818182</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -2752,7 +2752,7 @@
         <v>112</v>
       </c>
       <c r="B93">
-        <v>0.6321428571428571</v>
+        <v>0.584375</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -2760,7 +2760,7 @@
         <v>113</v>
       </c>
       <c r="B94">
-        <v>0.643979057591623</v>
+        <v>0.6129032258064516</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -2768,7 +2768,7 @@
         <v>114</v>
       </c>
       <c r="B95">
-        <v>0.5098039215686274</v>
+        <v>0.4743589743589743</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -2776,7 +2776,7 @@
         <v>115</v>
       </c>
       <c r="B96">
-        <v>0.6959459459459459</v>
+        <v>0.653179190751445</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -2784,7 +2784,7 @@
         <v>116</v>
       </c>
       <c r="B97">
-        <v>0.5295774647887324</v>
+        <v>0.4753694581280788</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -2792,7 +2792,7 @@
         <v>117</v>
       </c>
       <c r="B98">
-        <v>0.5323529411764706</v>
+        <v>0.4819587628865979</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -2800,7 +2800,7 @@
         <v>118</v>
       </c>
       <c r="B99">
-        <v>0.2561853351327035</v>
+        <v>0.2157190635451505</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -2808,7 +2808,7 @@
         <v>119</v>
       </c>
       <c r="B100">
-        <v>0.6166666666666667</v>
+        <v>0.5656934306569343</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -2816,7 +2816,7 @@
         <v>120</v>
       </c>
       <c r="B101">
-        <v>0.6030927835051546</v>
+        <v>0.5462555066079295</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -2824,7 +2824,7 @@
         <v>121</v>
       </c>
       <c r="B102">
-        <v>0.5229759299781181</v>
+        <v>0.4689265536723164</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -2832,7 +2832,7 @@
         <v>122</v>
       </c>
       <c r="B103">
-        <v>0.6625</v>
+        <v>0.6236559139784946</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -2840,7 +2840,7 @@
         <v>123</v>
       </c>
       <c r="B104">
-        <v>0.2544209925841415</v>
+        <v>0.2279046673286991</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -2848,7 +2848,7 @@
         <v>124</v>
       </c>
       <c r="B105">
-        <v>0.4700598802395209</v>
+        <v>0.4234693877551021</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -2856,7 +2856,7 @@
         <v>125</v>
       </c>
       <c r="B106">
-        <v>0.72</v>
+        <v>0.6686046511627907</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -2864,7 +2864,7 @@
         <v>126</v>
       </c>
       <c r="B107">
-        <v>0.3758556316116988</v>
+        <v>0.3367791077257889</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -2872,7 +2872,7 @@
         <v>127</v>
       </c>
       <c r="B108">
-        <v>0.4715302491103203</v>
+        <v>0.4279141104294479</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -2880,7 +2880,7 @@
         <v>128</v>
       </c>
       <c r="B109">
-        <v>0.5596707818930041</v>
+        <v>0.5124555160142349</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -2888,7 +2888,7 @@
         <v>129</v>
       </c>
       <c r="B110">
-        <v>0.4509803921568628</v>
+        <v>0.4020752269779507</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -2896,7 +2896,7 @@
         <v>130</v>
       </c>
       <c r="B111">
-        <v>0.5586206896551724</v>
+        <v>0.5114942528735632</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -2904,7 +2904,7 @@
         <v>131</v>
       </c>
       <c r="B112">
-        <v>0.5982142857142857</v>
+        <v>0.5338345864661654</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -2912,7 +2912,7 @@
         <v>132</v>
       </c>
       <c r="B113">
-        <v>0.4810126582278481</v>
+        <v>0.446866485013624</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -2920,7 +2920,7 @@
         <v>133</v>
       </c>
       <c r="B114">
-        <v>0.59375</v>
+        <v>0.5270758122743683</v>
       </c>
     </row>
   </sheetData>
@@ -2949,7 +2949,7 @@
         <v>134</v>
       </c>
       <c r="B2">
-        <v>0.6666666666666666</v>
+        <v>0.5671641791044776</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2957,7 +2957,7 @@
         <v>135</v>
       </c>
       <c r="B3">
-        <v>0.5490654205607477</v>
+        <v>0.4665391969407266</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2965,7 +2965,7 @@
         <v>136</v>
       </c>
       <c r="B4">
-        <v>0.6666666666666666</v>
+        <v>0.639344262295082</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2973,7 +2973,7 @@
         <v>137</v>
       </c>
       <c r="B5">
-        <v>0.4326599326599326</v>
+        <v>0.3802716225875625</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2981,7 +2981,7 @@
         <v>138</v>
       </c>
       <c r="B6">
-        <v>0.4659300184162062</v>
+        <v>0.4213036565977742</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2989,7 +2989,7 @@
         <v>139</v>
       </c>
       <c r="B7">
-        <v>0.5014245014245015</v>
+        <v>0.4358353510895884</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2997,7 +2997,7 @@
         <v>140</v>
       </c>
       <c r="B8">
-        <v>0.2930899096976836</v>
+        <v>0.2547866980181391</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -3005,7 +3005,7 @@
         <v>141</v>
       </c>
       <c r="B9">
-        <v>0.3434343434343434</v>
+        <v>0.2997542997542997</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3013,7 +3013,7 @@
         <v>142</v>
       </c>
       <c r="B10">
-        <v>0.4209183673469388</v>
+        <v>0.3815350389321469</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -3021,7 +3021,7 @@
         <v>143</v>
       </c>
       <c r="B11">
-        <v>0.3851944792973651</v>
+        <v>0.3522975929978118</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3029,7 +3029,7 @@
         <v>144</v>
       </c>
       <c r="B12">
-        <v>0.4466666666666667</v>
+        <v>0.3994293865905849</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -3037,7 +3037,7 @@
         <v>145</v>
       </c>
       <c r="B13">
-        <v>0.4824707846410685</v>
+        <v>0.4329004329004329</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -3045,7 +3045,7 @@
         <v>146</v>
       </c>
       <c r="B14">
-        <v>0.7083333333333334</v>
+        <v>0.6811594202898551</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -3053,7 +3053,7 @@
         <v>147</v>
       </c>
       <c r="B15">
-        <v>0.5454545454545454</v>
+        <v>0.4961240310077519</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3061,7 +3061,7 @@
         <v>148</v>
       </c>
       <c r="B16">
-        <v>0.6287425149700598</v>
+        <v>0.5885416666666666</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -3069,7 +3069,7 @@
         <v>149</v>
       </c>
       <c r="B17">
-        <v>0.4261261261261261</v>
+        <v>0.3795275590551181</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -3077,7 +3077,7 @@
         <v>150</v>
       </c>
       <c r="B18">
-        <v>0.4263059701492538</v>
+        <v>0.3789731051344744</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -3085,7 +3085,7 @@
         <v>151</v>
       </c>
       <c r="B19">
-        <v>0.4353182751540041</v>
+        <v>0.4084249084249084</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -3093,7 +3093,7 @@
         <v>152</v>
       </c>
       <c r="B20">
-        <v>0.5223880597014925</v>
+        <v>0.4704944178628389</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -3101,7 +3101,7 @@
         <v>153</v>
       </c>
       <c r="B21">
-        <v>0.5208333333333334</v>
+        <v>0.4905660377358491</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -3109,7 +3109,7 @@
         <v>154</v>
       </c>
       <c r="B22">
-        <v>0.3195342820181112</v>
+        <v>0.2974828375286041</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -3117,7 +3117,7 @@
         <v>155</v>
       </c>
       <c r="B23">
-        <v>0.3619271445358402</v>
+        <v>0.2948717948717949</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -3125,7 +3125,7 @@
         <v>156</v>
       </c>
       <c r="B24">
-        <v>0.5095238095238095</v>
+        <v>0.4819277108433735</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -3133,7 +3133,7 @@
         <v>157</v>
       </c>
       <c r="B25">
-        <v>0.3665158371040724</v>
+        <v>0.3268292682926829</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -3141,7 +3141,7 @@
         <v>158</v>
       </c>
       <c r="B26">
-        <v>0.5152671755725191</v>
+        <v>0.4491114701130856</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -3149,7 +3149,7 @@
         <v>159</v>
       </c>
       <c r="B27">
-        <v>0.4410958904109589</v>
+        <v>0.3899082568807339</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -3157,7 +3157,7 @@
         <v>160</v>
       </c>
       <c r="B28">
-        <v>0.6796116504854369</v>
+        <v>0.6129032258064516</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -3165,7 +3165,7 @@
         <v>161</v>
       </c>
       <c r="B29">
-        <v>0.4968847352024922</v>
+        <v>0.4481830417227456</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -3173,7 +3173,7 @@
         <v>162</v>
       </c>
       <c r="B30">
-        <v>0.4705882352941176</v>
+        <v>0.4548872180451128</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -3181,7 +3181,7 @@
         <v>163</v>
       </c>
       <c r="B31">
-        <v>0.5531135531135531</v>
+        <v>0.4953560371517028</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -3189,7 +3189,7 @@
         <v>164</v>
       </c>
       <c r="B32">
-        <v>0.3965141612200436</v>
+        <v>0.3353221957040573</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -3197,7 +3197,7 @@
         <v>165</v>
       </c>
       <c r="B33">
-        <v>0.4074074074074074</v>
+        <v>0.3542074363992172</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -3205,7 +3205,7 @@
         <v>166</v>
       </c>
       <c r="B34">
-        <v>0.553921568627451</v>
+        <v>0.4938271604938271</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -3213,7 +3213,7 @@
         <v>167</v>
       </c>
       <c r="B35">
-        <v>0.4089219330855018</v>
+        <v>0.3666666666666666</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -3221,7 +3221,7 @@
         <v>168</v>
       </c>
       <c r="B36">
-        <v>0.5896805896805897</v>
+        <v>0.500998003992016</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -3229,7 +3229,7 @@
         <v>169</v>
       </c>
       <c r="B37">
-        <v>0.5257903494176372</v>
+        <v>0.4586894586894587</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -3237,7 +3237,7 @@
         <v>170</v>
       </c>
       <c r="B38">
-        <v>0.4898989898989899</v>
+        <v>0.4411134903640257</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -3245,7 +3245,7 @@
         <v>171</v>
       </c>
       <c r="B39">
-        <v>0.5032679738562091</v>
+        <v>0.4634831460674158</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -3253,7 +3253,7 @@
         <v>172</v>
       </c>
       <c r="B40">
-        <v>0.4894894894894895</v>
+        <v>0.4587912087912088</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -3261,7 +3261,7 @@
         <v>173</v>
       </c>
       <c r="B41">
-        <v>0.462046204620462</v>
+        <v>0.4261645193260654</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -3269,7 +3269,7 @@
         <v>174</v>
       </c>
       <c r="B42">
-        <v>0.3808510638297872</v>
+        <v>0.3436928702010969</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -3277,7 +3277,7 @@
         <v>175</v>
       </c>
       <c r="B43">
-        <v>0.3892857142857143</v>
+        <v>0.3497757847533632</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -3285,7 +3285,7 @@
         <v>176</v>
       </c>
       <c r="B44">
-        <v>0.5517241379310345</v>
+        <v>0.4854881266490765</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -3293,7 +3293,7 @@
         <v>177</v>
       </c>
       <c r="B45">
-        <v>0.3724489795918368</v>
+        <v>0.3391107761868877</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -3301,7 +3301,7 @@
         <v>178</v>
       </c>
       <c r="B46">
-        <v>0.4794816414686825</v>
+        <v>0.4187725631768953</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -3317,7 +3317,7 @@
         <v>180</v>
       </c>
       <c r="B48">
-        <v>0.4594594594594595</v>
+        <v>0.4127423822714681</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3325,7 +3325,7 @@
         <v>181</v>
       </c>
       <c r="B49">
-        <v>0.5777777777777777</v>
+        <v>0.5092936802973977</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3333,7 +3333,7 @@
         <v>182</v>
       </c>
       <c r="B50">
-        <v>0.4952681388012618</v>
+        <v>0.438692098092643</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3341,7 +3341,7 @@
         <v>183</v>
       </c>
       <c r="B51">
-        <v>0.5463414634146342</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -3349,7 +3349,7 @@
         <v>184</v>
       </c>
       <c r="B52">
-        <v>0.5907172995780591</v>
+        <v>0.5321428571428571</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -3357,7 +3357,7 @@
         <v>185</v>
       </c>
       <c r="B53">
-        <v>0.7125748502994012</v>
+        <v>0.6564102564102564</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -3365,7 +3365,7 @@
         <v>186</v>
       </c>
       <c r="B54">
-        <v>0.3785714285714286</v>
+        <v>0.3478260869565217</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -3373,7 +3373,7 @@
         <v>187</v>
       </c>
       <c r="B55">
-        <v>0.5423728813559322</v>
+        <v>0.5010570824524313</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -3381,7 +3381,7 @@
         <v>188</v>
       </c>
       <c r="B56">
-        <v>0.5137111517367459</v>
+        <v>0.4504643962848297</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -3389,7 +3389,7 @@
         <v>189</v>
       </c>
       <c r="B57">
-        <v>0.2995066948555321</v>
+        <v>0.2757097791798107</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -3397,7 +3397,7 @@
         <v>190</v>
       </c>
       <c r="B58">
-        <v>0.4159021406727829</v>
+        <v>0.3748361730013106</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -3405,7 +3405,7 @@
         <v>191</v>
       </c>
       <c r="B59">
-        <v>0.398406374501992</v>
+        <v>0.3418940609951846</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -3413,7 +3413,7 @@
         <v>192</v>
       </c>
       <c r="B60">
-        <v>0.5650557620817844</v>
+        <v>0.5063694267515924</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -3421,7 +3421,7 @@
         <v>193</v>
       </c>
       <c r="B61">
-        <v>0.3293539325842696</v>
+        <v>0.291868932038835</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -3429,7 +3429,7 @@
         <v>194</v>
       </c>
       <c r="B62">
-        <v>0.3779036827195467</v>
+        <v>0.3237103644107903</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -3437,7 +3437,7 @@
         <v>195</v>
       </c>
       <c r="B63">
-        <v>0.4906832298136646</v>
+        <v>0.4423592493297587</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -3445,7 +3445,7 @@
         <v>196</v>
       </c>
       <c r="B64">
-        <v>0.3171690694626474</v>
+        <v>0.2854413450515858</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -3453,7 +3453,7 @@
         <v>197</v>
       </c>
       <c r="B65">
-        <v>0.6153846153846154</v>
+        <v>0.5722222222222222</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -3461,7 +3461,7 @@
         <v>198</v>
       </c>
       <c r="B66">
-        <v>0.5009560229445507</v>
+        <v>0.4514003294892916</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -3469,7 +3469,7 @@
         <v>199</v>
       </c>
       <c r="B67">
-        <v>0.6052631578947368</v>
+        <v>0.5447761194029851</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -3477,7 +3477,7 @@
         <v>200</v>
       </c>
       <c r="B68">
-        <v>0.3612535612535612</v>
+        <v>0.3191699604743083</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -3485,7 +3485,7 @@
         <v>201</v>
       </c>
       <c r="B69">
-        <v>0.3674641148325359</v>
+        <v>0.3252032520325203</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -3493,7 +3493,7 @@
         <v>202</v>
       </c>
       <c r="B70">
-        <v>0.5975103734439834</v>
+        <v>0.4635568513119533</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -3501,7 +3501,7 @@
         <v>203</v>
       </c>
       <c r="B71">
-        <v>0.4481765834932822</v>
+        <v>0.3645990922844176</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -3509,7 +3509,7 @@
         <v>204</v>
       </c>
       <c r="B72">
-        <v>0.3276216586703221</v>
+        <v>0.2718767198679141</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -3517,7 +3517,7 @@
         <v>205</v>
       </c>
       <c r="B73">
-        <v>0.675</v>
+        <v>0.6153846153846154</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -3525,7 +3525,7 @@
         <v>206</v>
       </c>
       <c r="B74">
-        <v>0.215076660988075</v>
+        <v>0.1934171597633136</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -3533,7 +3533,7 @@
         <v>207</v>
       </c>
       <c r="B75">
-        <v>0.8461538461538461</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -3541,7 +3541,7 @@
         <v>208</v>
       </c>
       <c r="B76">
-        <v>0.6466666666666666</v>
+        <v>0.5977011494252874</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -3549,7 +3549,7 @@
         <v>209</v>
       </c>
       <c r="B77">
-        <v>0.3759590792838874</v>
+        <v>0.3352626892252894</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -3557,7 +3557,7 @@
         <v>210</v>
       </c>
       <c r="B78">
-        <v>0.2818745692625775</v>
+        <v>0.2374647887323944</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -3565,7 +3565,7 @@
         <v>211</v>
       </c>
       <c r="B79">
-        <v>0.4766949152542373</v>
+        <v>0.4213381555153707</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -3573,7 +3573,7 @@
         <v>212</v>
       </c>
       <c r="B80">
-        <v>0.4740484429065744</v>
+        <v>0.4236526946107784</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3581,7 +3581,7 @@
         <v>213</v>
       </c>
       <c r="B81">
-        <v>0.480672268907563</v>
+        <v>0.4344624447717231</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3589,7 +3589,7 @@
         <v>214</v>
       </c>
       <c r="B82">
-        <v>0.465979381443299</v>
+        <v>0.4033333333333333</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3597,7 +3597,7 @@
         <v>215</v>
       </c>
       <c r="B83">
-        <v>0.717948717948718</v>
+        <v>0.6559139784946236</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -3605,7 +3605,7 @@
         <v>216</v>
       </c>
       <c r="B84">
-        <v>0.7560975609756098</v>
+        <v>0.6981132075471698</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -3613,7 +3613,7 @@
         <v>217</v>
       </c>
       <c r="B85">
-        <v>0.4989648033126294</v>
+        <v>0.4158415841584158</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -3621,7 +3621,7 @@
         <v>218</v>
       </c>
       <c r="B86">
-        <v>0.5059021922428331</v>
+        <v>0.4368932038834951</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -3629,7 +3629,7 @@
         <v>219</v>
       </c>
       <c r="B87">
-        <v>0.4360902255639098</v>
+        <v>0.3850931677018634</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -3637,7 +3637,7 @@
         <v>220</v>
       </c>
       <c r="B88">
-        <v>0.5151515151515151</v>
+        <v>0.4701195219123506</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -3645,7 +3645,7 @@
         <v>221</v>
       </c>
       <c r="B89">
-        <v>0.5269709543568465</v>
+        <v>0.4927536231884058</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -3653,7 +3653,7 @@
         <v>222</v>
       </c>
       <c r="B90">
-        <v>0.4651600753295669</v>
+        <v>0.4042879019908117</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -3661,7 +3661,7 @@
         <v>223</v>
       </c>
       <c r="B91">
-        <v>0.6896551724137931</v>
+        <v>0.6521739130434783</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -3669,7 +3669,7 @@
         <v>224</v>
       </c>
       <c r="B92">
-        <v>0.4368482039397451</v>
+        <v>0.4014300306435138</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -3677,7 +3677,7 @@
         <v>225</v>
       </c>
       <c r="B93">
-        <v>0.5301587301587302</v>
+        <v>0.4767123287671233</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -3685,7 +3685,7 @@
         <v>226</v>
       </c>
       <c r="B94">
-        <v>0.4712153518123667</v>
+        <v>0.4066317626527051</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -3693,7 +3693,7 @@
         <v>227</v>
       </c>
       <c r="B95">
-        <v>0.5608308605341247</v>
+        <v>0.46875</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -3701,7 +3701,7 @@
         <v>228</v>
       </c>
       <c r="B96">
-        <v>0.4166666666666667</v>
+        <v>0.3676646706586826</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -3709,7 +3709,7 @@
         <v>229</v>
       </c>
       <c r="B97">
-        <v>0.6521739130434783</v>
+        <v>0.5697674418604651</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -3717,7 +3717,7 @@
         <v>230</v>
       </c>
       <c r="B98">
-        <v>0.554006968641115</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -3725,7 +3725,7 @@
         <v>231</v>
       </c>
       <c r="B99">
-        <v>0.5294117647058824</v>
+        <v>0.4887640449438202</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -3733,7 +3733,7 @@
         <v>232</v>
       </c>
       <c r="B100">
-        <v>0.487603305785124</v>
+        <v>0.4391534391534391</v>
       </c>
     </row>
     <row r="101" spans="1:2">
@@ -3741,7 +3741,7 @@
         <v>233</v>
       </c>
       <c r="B101">
-        <v>0.4257950530035335</v>
+        <v>0.3841463414634146</v>
       </c>
     </row>
     <row r="102" spans="1:2">
@@ -3749,7 +3749,7 @@
         <v>234</v>
       </c>
       <c r="B102">
-        <v>0.529296875</v>
+        <v>0.4528</v>
       </c>
     </row>
     <row r="103" spans="1:2">
@@ -3757,7 +3757,7 @@
         <v>235</v>
       </c>
       <c r="B103">
-        <v>0.3817427385892116</v>
+        <v>0.3535980148883375</v>
       </c>
     </row>
     <row r="104" spans="1:2">
@@ -3765,7 +3765,7 @@
         <v>236</v>
       </c>
       <c r="B104">
-        <v>0.4638694638694639</v>
+        <v>0.4183266932270917</v>
       </c>
     </row>
     <row r="105" spans="1:2">
@@ -3773,7 +3773,7 @@
         <v>237</v>
       </c>
       <c r="B105">
-        <v>0.5855670103092784</v>
+        <v>0.5384615384615384</v>
       </c>
     </row>
     <row r="106" spans="1:2">
@@ -3781,7 +3781,7 @@
         <v>238</v>
       </c>
       <c r="B106">
-        <v>0.5934959349593496</v>
+        <v>0.5693430656934306</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -3789,7 +3789,7 @@
         <v>239</v>
       </c>
       <c r="B107">
-        <v>0.5686274509803921</v>
+        <v>0.5391304347826087</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -3797,7 +3797,7 @@
         <v>240</v>
       </c>
       <c r="B108">
-        <v>0.2926430517711172</v>
+        <v>0.2577464788732394</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -3805,7 +3805,7 @@
         <v>241</v>
       </c>
       <c r="B109">
-        <v>0.66</v>
+        <v>0.6206896551724138</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -3813,7 +3813,7 @@
         <v>242</v>
       </c>
       <c r="B110">
-        <v>0.4482306684141547</v>
+        <v>0.4071100917431192</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -3821,7 +3821,7 @@
         <v>243</v>
       </c>
       <c r="B111">
-        <v>0.4080389768574909</v>
+        <v>0.3608786610878661</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -3829,7 +3829,7 @@
         <v>244</v>
       </c>
       <c r="B112">
-        <v>0.76</v>
+        <v>0.7543859649122807</v>
       </c>
     </row>
     <row r="113" spans="1:2">
@@ -3837,7 +3837,7 @@
         <v>245</v>
       </c>
       <c r="B113">
-        <v>0.4662698412698413</v>
+        <v>0.3944353518821604</v>
       </c>
     </row>
     <row r="114" spans="1:2">
@@ -3845,7 +3845,7 @@
         <v>246</v>
       </c>
       <c r="B114">
-        <v>0.4853273137697517</v>
+        <v>0.436046511627907</v>
       </c>
     </row>
     <row r="115" spans="1:2">
@@ -3853,7 +3853,7 @@
         <v>247</v>
       </c>
       <c r="B115">
-        <v>0.475177304964539</v>
+        <v>0.4250513347022588</v>
       </c>
     </row>
     <row r="116" spans="1:2">
@@ -3861,7 +3861,7 @@
         <v>248</v>
       </c>
       <c r="B116">
-        <v>0.554016620498615</v>
+        <v>0.4988066825775656</v>
       </c>
     </row>
     <row r="117" spans="1:2">
@@ -3869,7 +3869,7 @@
         <v>249</v>
       </c>
       <c r="B117">
-        <v>0.5242070116861436</v>
+        <v>0.4594594594594595</v>
       </c>
     </row>
     <row r="118" spans="1:2">
@@ -3877,7 +3877,7 @@
         <v>250</v>
       </c>
       <c r="B118">
-        <v>0.5205811138014528</v>
+        <v>0.4680412371134021</v>
       </c>
     </row>
     <row r="119" spans="1:2">
@@ -3885,7 +3885,7 @@
         <v>251</v>
       </c>
       <c r="B119">
-        <v>0.507908611599297</v>
+        <v>0.4417910447761194</v>
       </c>
     </row>
     <row r="120" spans="1:2">
@@ -3893,7 +3893,7 @@
         <v>252</v>
       </c>
       <c r="B120">
-        <v>0.4790286975717439</v>
+        <v>0.4326375711574952</v>
       </c>
     </row>
     <row r="121" spans="1:2">
@@ -3901,7 +3901,7 @@
         <v>253</v>
       </c>
       <c r="B121">
-        <v>0.5188536953242836</v>
+        <v>0.4471337579617835</v>
       </c>
     </row>
     <row r="122" spans="1:2">
@@ -3909,7 +3909,7 @@
         <v>254</v>
       </c>
       <c r="B122">
-        <v>0.5259515570934256</v>
+        <v>0.4064837905236908</v>
       </c>
     </row>
     <row r="123" spans="1:2">
@@ -3917,7 +3917,7 @@
         <v>255</v>
       </c>
       <c r="B123">
-        <v>0.5580589254766031</v>
+        <v>0.4962292609351433</v>
       </c>
     </row>
     <row r="124" spans="1:2">
@@ -3925,7 +3925,7 @@
         <v>256</v>
       </c>
       <c r="B124">
-        <v>0.5604026845637584</v>
+        <v>0.5144508670520231</v>
       </c>
     </row>
     <row r="125" spans="1:2">
@@ -3933,7 +3933,7 @@
         <v>257</v>
       </c>
       <c r="B125">
-        <v>0.3843236409608091</v>
+        <v>0.3393617021276596</v>
       </c>
     </row>
     <row r="126" spans="1:2">
@@ -3941,7 +3941,7 @@
         <v>258</v>
       </c>
       <c r="B126">
-        <v>0.4733840304182509</v>
+        <v>0.4096774193548387</v>
       </c>
     </row>
     <row r="127" spans="1:2">
@@ -3949,7 +3949,7 @@
         <v>259</v>
       </c>
       <c r="B127">
-        <v>0.5681233933161953</v>
+        <v>0.509719222462203</v>
       </c>
     </row>
     <row r="128" spans="1:2">
@@ -3957,7 +3957,7 @@
         <v>260</v>
       </c>
       <c r="B128">
-        <v>0.5121951219512195</v>
+        <v>0.4541284403669725</v>
       </c>
     </row>
     <row r="129" spans="1:2">
@@ -3965,7 +3965,7 @@
         <v>261</v>
       </c>
       <c r="B129">
-        <v>0.526984126984127</v>
+        <v>0.4522875816993464</v>
       </c>
     </row>
     <row r="130" spans="1:2">
@@ -3973,7 +3973,7 @@
         <v>262</v>
       </c>
       <c r="B130">
-        <v>0.8125</v>
+        <v>0.7931034482758621</v>
       </c>
     </row>
     <row r="131" spans="1:2">
@@ -3981,7 +3981,7 @@
         <v>263</v>
       </c>
       <c r="B131">
-        <v>0.4416562107904642</v>
+        <v>0.3866809881847476</v>
       </c>
     </row>
     <row r="132" spans="1:2">
@@ -3989,7 +3989,7 @@
         <v>264</v>
       </c>
       <c r="B132">
-        <v>0.6257309941520468</v>
+        <v>0.572139303482587</v>
       </c>
     </row>
     <row r="133" spans="1:2">
@@ -3997,7 +3997,7 @@
         <v>265</v>
       </c>
       <c r="B133">
-        <v>0.5854214123006833</v>
+        <v>0.5155642023346303</v>
       </c>
     </row>
     <row r="134" spans="1:2">
@@ -4005,7 +4005,7 @@
         <v>266</v>
       </c>
       <c r="B134">
-        <v>0.3754716981132076</v>
+        <v>0.3357664233576642</v>
       </c>
     </row>
     <row r="135" spans="1:2">
@@ -4013,7 +4013,7 @@
         <v>267</v>
       </c>
       <c r="B135">
-        <v>0.7560975609756098</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="136" spans="1:2">
@@ -4021,7 +4021,7 @@
         <v>268</v>
       </c>
       <c r="B136">
-        <v>0.5714285714285714</v>
+        <v>0.55</v>
       </c>
     </row>
     <row r="137" spans="1:2">
@@ -4029,7 +4029,7 @@
         <v>269</v>
       </c>
       <c r="B137">
-        <v>0.481149012567325</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="138" spans="1:2">
@@ -4037,7 +4037,7 @@
         <v>270</v>
       </c>
       <c r="B138">
-        <v>0.5967741935483871</v>
+        <v>0.5201342281879194</v>
       </c>
     </row>
     <row r="139" spans="1:2">
@@ -4045,7 +4045,7 @@
         <v>271</v>
       </c>
       <c r="B139">
-        <v>0.6642335766423357</v>
+        <v>0.6339869281045751</v>
       </c>
     </row>
     <row r="140" spans="1:2">
@@ -4053,7 +4053,7 @@
         <v>272</v>
       </c>
       <c r="B140">
-        <v>0.4095127610208817</v>
+        <v>0.357487922705314</v>
       </c>
     </row>
     <row r="141" spans="1:2">
@@ -4061,7 +4061,7 @@
         <v>273</v>
       </c>
       <c r="B141">
-        <v>0.6239316239316239</v>
+        <v>0.5467625899280576</v>
       </c>
     </row>
     <row r="142" spans="1:2">
@@ -4069,7 +4069,7 @@
         <v>274</v>
       </c>
       <c r="B142">
-        <v>0.5964285714285714</v>
+        <v>0.5306748466257669</v>
       </c>
     </row>
     <row r="143" spans="1:2">
@@ -4077,7 +4077,7 @@
         <v>275</v>
       </c>
       <c r="B143">
-        <v>0.5366242038216561</v>
+        <v>0.4698630136986301</v>
       </c>
     </row>
     <row r="144" spans="1:2">
@@ -4085,7 +4085,7 @@
         <v>276</v>
       </c>
       <c r="B144">
-        <v>0.4847222222222222</v>
+        <v>0.4330900243309003</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -4093,7 +4093,7 @@
         <v>277</v>
       </c>
       <c r="B145">
-        <v>0.6024464831804281</v>
+        <v>0.5435356200527705</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -4101,7 +4101,7 @@
         <v>278</v>
       </c>
       <c r="B146">
-        <v>0.5347490347490348</v>
+        <v>0.4614147909967846</v>
       </c>
     </row>
     <row r="147" spans="1:2">
@@ -4109,7 +4109,7 @@
         <v>279</v>
       </c>
       <c r="B147">
-        <v>0.3483735571878279</v>
+        <v>0.3052351375332742</v>
       </c>
     </row>
     <row r="148" spans="1:2">
@@ -4117,7 +4117,7 @@
         <v>280</v>
       </c>
       <c r="B148">
-        <v>0.5073891625615764</v>
+        <v>0.4557235421166307</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -4125,7 +4125,7 @@
         <v>281</v>
       </c>
       <c r="B149">
-        <v>0.7058823529411765</v>
+        <v>0.6474358974358975</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -4133,7 +4133,7 @@
         <v>282</v>
       </c>
       <c r="B150">
-        <v>0.3274144651364227</v>
+        <v>0.2831369661266568</v>
       </c>
     </row>
     <row r="151" spans="1:2">
@@ -4141,7 +4141,7 @@
         <v>283</v>
       </c>
       <c r="B151">
-        <v>0.4959785522788204</v>
+        <v>0.4439359267734554</v>
       </c>
     </row>
     <row r="152" spans="1:2">
@@ -4149,7 +4149,7 @@
         <v>284</v>
       </c>
       <c r="B152">
-        <v>0.9210526315789473</v>
+        <v>0.9069767441860465</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -4157,7 +4157,7 @@
         <v>285</v>
       </c>
       <c r="B153">
-        <v>0.6210526315789474</v>
+        <v>0.5709876543209876</v>
       </c>
     </row>
   </sheetData>
@@ -4186,7 +4186,7 @@
         <v>286</v>
       </c>
       <c r="B2">
-        <v>0.6270270270270271</v>
+        <v>0.5701357466063348</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4194,7 +4194,7 @@
         <v>287</v>
       </c>
       <c r="B3">
-        <v>0.5572755417956656</v>
+        <v>0.5179063360881543</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4202,7 +4202,7 @@
         <v>288</v>
       </c>
       <c r="B4">
-        <v>0.5435356200527705</v>
+        <v>0.5083135391923991</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4210,7 +4210,7 @@
         <v>289</v>
       </c>
       <c r="B5">
-        <v>0.9285714285714286</v>
+        <v>0.8936170212765957</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4218,7 +4218,7 @@
         <v>290</v>
       </c>
       <c r="B6">
-        <v>0.3929098966026588</v>
+        <v>0.3004338394793926</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4226,7 +4226,7 @@
         <v>291</v>
       </c>
       <c r="B7">
-        <v>0.4260614934114202</v>
+        <v>0.3728606356968215</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4234,7 +4234,7 @@
         <v>292</v>
       </c>
       <c r="B8">
-        <v>0.4474885844748858</v>
+        <v>0.3853904282115869</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4242,7 +4242,7 @@
         <v>293</v>
       </c>
       <c r="B9">
-        <v>0.433641975308642</v>
+        <v>0.3803921568627451</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4250,7 +4250,7 @@
         <v>294</v>
       </c>
       <c r="B10">
-        <v>0.591304347826087</v>
+        <v>0.5509433962264151</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4258,7 +4258,7 @@
         <v>295</v>
       </c>
       <c r="B11">
-        <v>0.2475538160469667</v>
+        <v>0.2194513715710723</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4266,7 +4266,7 @@
         <v>296</v>
       </c>
       <c r="B12">
-        <v>0.2735483870967742</v>
+        <v>0.250575594781274</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4274,7 +4274,7 @@
         <v>297</v>
       </c>
       <c r="B13">
-        <v>0.4717948717948718</v>
+        <v>0.4311377245508982</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4282,7 +4282,7 @@
         <v>298</v>
       </c>
       <c r="B14">
-        <v>0.440536013400335</v>
+        <v>0.3926031294452347</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4290,7 +4290,7 @@
         <v>299</v>
       </c>
       <c r="B15">
-        <v>0.3722304283604136</v>
+        <v>0.3201970443349754</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4298,7 +4298,7 @@
         <v>300</v>
       </c>
       <c r="B16">
-        <v>0.5763546798029556</v>
+        <v>0.5387931034482759</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4306,7 +4306,7 @@
         <v>301</v>
       </c>
       <c r="B17">
-        <v>0.425273390036452</v>
+        <v>0.3715455475946776</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4314,7 +4314,7 @@
         <v>302</v>
       </c>
       <c r="B18">
-        <v>0.4433962264150944</v>
+        <v>0.3750748951467945</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4322,7 +4322,7 @@
         <v>303</v>
       </c>
       <c r="B19">
-        <v>0.5228915662650603</v>
+        <v>0.4690082644628099</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4330,7 +4330,7 @@
         <v>304</v>
       </c>
       <c r="B20">
-        <v>0.5619335347432024</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4338,7 +4338,7 @@
         <v>305</v>
       </c>
       <c r="B21">
-        <v>0.5719769673704415</v>
+        <v>0.4849921011058452</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4346,7 +4346,7 @@
         <v>306</v>
       </c>
       <c r="B22">
-        <v>0.4731585518102372</v>
+        <v>0.418554476806904</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4354,7 +4354,7 @@
         <v>307</v>
       </c>
       <c r="B23">
-        <v>0.4697286012526096</v>
+        <v>0.4319852941176471</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4362,7 +4362,7 @@
         <v>308</v>
       </c>
       <c r="B24">
-        <v>0.2601156069364162</v>
+        <v>0.2265825281009663</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4370,7 +4370,7 @@
         <v>309</v>
       </c>
       <c r="B25">
-        <v>0.3012106537530266</v>
+        <v>0.2589285714285715</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4378,7 +4378,7 @@
         <v>310</v>
       </c>
       <c r="B26">
-        <v>0.4229390681003584</v>
+        <v>0.3290155440414508</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4386,7 +4386,7 @@
         <v>311</v>
       </c>
       <c r="B27">
-        <v>0.4945054945054945</v>
+        <v>0.4239130434782609</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -4394,7 +4394,7 @@
         <v>312</v>
       </c>
       <c r="B28">
-        <v>0.4407345575959933</v>
+        <v>0.3808219178082192</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -4402,7 +4402,7 @@
         <v>313</v>
       </c>
       <c r="B29">
-        <v>0.5325077399380805</v>
+        <v>0.4535031847133758</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -4410,7 +4410,7 @@
         <v>314</v>
       </c>
       <c r="B30">
-        <v>0.4547038327526132</v>
+        <v>0.3819918144611187</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -4418,7 +4418,7 @@
         <v>315</v>
       </c>
       <c r="B31">
-        <v>0.6706586826347305</v>
+        <v>0.6230366492146597</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -4426,7 +4426,7 @@
         <v>316</v>
       </c>
       <c r="B32">
-        <v>0.4604200323101777</v>
+        <v>0.4051841746248295</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -4434,7 +4434,7 @@
         <v>317</v>
       </c>
       <c r="B33">
-        <v>0.6273584905660378</v>
+        <v>0.5772357723577236</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -4442,7 +4442,7 @@
         <v>318</v>
       </c>
       <c r="B34">
-        <v>0.6011560693641619</v>
+        <v>0.5390243902439025</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -4450,7 +4450,7 @@
         <v>319</v>
       </c>
       <c r="B35">
-        <v>0.6568047337278107</v>
+        <v>0.616580310880829</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -4458,7 +4458,7 @@
         <v>320</v>
       </c>
       <c r="B36">
-        <v>0.3649564375605034</v>
+        <v>0.3160453808752026</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -4466,7 +4466,7 @@
         <v>321</v>
       </c>
       <c r="B37">
-        <v>0.5199063231850117</v>
+        <v>0.4512922465208747</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -4474,7 +4474,7 @@
         <v>322</v>
       </c>
       <c r="B38">
-        <v>0.3772972972972973</v>
+        <v>0.3249776186213071</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -4482,7 +4482,7 @@
         <v>323</v>
       </c>
       <c r="B39">
-        <v>0.4794117647058824</v>
+        <v>0.4203980099502487</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -4490,7 +4490,7 @@
         <v>324</v>
       </c>
       <c r="B40">
-        <v>0.5801526717557252</v>
+        <v>0.525</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -4498,7 +4498,7 @@
         <v>325</v>
       </c>
       <c r="B41">
-        <v>0.3677950594693504</v>
+        <v>0.3355102040816327</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -4506,7 +4506,7 @@
         <v>326</v>
       </c>
       <c r="B42">
-        <v>0.4585034013605442</v>
+        <v>0.4115566037735849</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -4514,7 +4514,7 @@
         <v>327</v>
       </c>
       <c r="B43">
-        <v>0.4581005586592179</v>
+        <v>0.4313725490196079</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -4522,7 +4522,7 @@
         <v>328</v>
       </c>
       <c r="B44">
-        <v>0.5905511811023622</v>
+        <v>0.5228758169934641</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -4530,7 +4530,7 @@
         <v>329</v>
       </c>
       <c r="B45">
-        <v>0.5672823218997362</v>
+        <v>0.4954954954954955</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -4538,7 +4538,7 @@
         <v>330</v>
       </c>
       <c r="B46">
-        <v>0.1692169216921692</v>
+        <v>0.1456928838951311</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -4546,7 +4546,7 @@
         <v>331</v>
       </c>
       <c r="B47">
-        <v>0.5853658536585366</v>
+        <v>0.5520833333333334</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -4554,7 +4554,7 @@
         <v>332</v>
       </c>
       <c r="B48">
-        <v>0.465979381443299</v>
+        <v>0.4301075268817204</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -4562,7 +4562,7 @@
         <v>333</v>
       </c>
       <c r="B49">
-        <v>0.6820809248554913</v>
+        <v>0.6510416666666666</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -4570,7 +4570,7 @@
         <v>334</v>
       </c>
       <c r="B50">
-        <v>0.3922413793103448</v>
+        <v>0.3476702508960574</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -4578,7 +4578,7 @@
         <v>335</v>
       </c>
       <c r="B51">
-        <v>0.3717434869739479</v>
+        <v>0.325938566552901</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -4586,7 +4586,7 @@
         <v>336</v>
       </c>
       <c r="B52">
-        <v>0.6633165829145728</v>
+        <v>0.6127659574468085</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -4594,7 +4594,7 @@
         <v>337</v>
       </c>
       <c r="B53">
-        <v>0.5664739884393064</v>
+        <v>0.5148514851485149</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -4602,7 +4602,7 @@
         <v>338</v>
       </c>
       <c r="B54">
-        <v>0.3823814133591481</v>
+        <v>0.3309178743961353</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -4610,7 +4610,7 @@
         <v>339</v>
       </c>
       <c r="B55">
-        <v>0.78</v>
+        <v>0.7818181818181819</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -4618,7 +4618,7 @@
         <v>340</v>
       </c>
       <c r="B56">
-        <v>0.4166666666666667</v>
+        <v>0.3746177370030581</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -4626,7 +4626,7 @@
         <v>341</v>
       </c>
       <c r="B57">
-        <v>0.3955119214586255</v>
+        <v>0.3419506462984724</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -4634,7 +4634,7 @@
         <v>342</v>
       </c>
       <c r="B58">
-        <v>0.4278768233387358</v>
+        <v>0.3959537572254335</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -4642,7 +4642,7 @@
         <v>343</v>
       </c>
       <c r="B59">
-        <v>0.591304347826087</v>
+        <v>0.5404411764705882</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -4650,7 +4650,7 @@
         <v>344</v>
       </c>
       <c r="B60">
-        <v>0.4058704453441296</v>
+        <v>0.3510548523206751</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -4658,7 +4658,7 @@
         <v>345</v>
       </c>
       <c r="B61">
-        <v>0.5669291338582677</v>
+        <v>0.5033112582781457</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -4666,7 +4666,7 @@
         <v>346</v>
       </c>
       <c r="B62">
-        <v>0.4725457570715474</v>
+        <v>0.4033149171270718</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -4674,7 +4674,7 @@
         <v>347</v>
       </c>
       <c r="B63">
-        <v>0.4260700389105058</v>
+        <v>0.3605015673981191</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -4682,7 +4682,7 @@
         <v>348</v>
       </c>
       <c r="B64">
-        <v>0.5221112696148359</v>
+        <v>0.4592952612393681</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -4690,7 +4690,7 @@
         <v>349</v>
       </c>
       <c r="B65">
-        <v>0.1972853535353535</v>
+        <v>0.1778393351800554</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -4698,7 +4698,7 @@
         <v>350</v>
       </c>
       <c r="B66">
-        <v>0.4869358669833729</v>
+        <v>0.4354838709677419</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -4706,7 +4706,7 @@
         <v>351</v>
       </c>
       <c r="B67">
-        <v>0.5270541082164328</v>
+        <v>0.4631217838765009</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -4714,7 +4714,7 @@
         <v>352</v>
       </c>
       <c r="B68">
-        <v>0.5033039647577092</v>
+        <v>0.4344186046511628</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -4722,7 +4722,7 @@
         <v>353</v>
       </c>
       <c r="B69">
-        <v>0.1911764705882353</v>
+        <v>0.1688085384447833</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -4730,7 +4730,7 @@
         <v>354</v>
       </c>
       <c r="B70">
-        <v>0.9130434782608695</v>
+        <v>0.8846153846153846</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -4738,7 +4738,7 @@
         <v>355</v>
       </c>
       <c r="B71">
-        <v>0.3950777202072539</v>
+        <v>0.343042071197411</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -4746,7 +4746,7 @@
         <v>356</v>
       </c>
       <c r="B72">
-        <v>0.4204819277108434</v>
+        <v>0.3685831622176591</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -4754,7 +4754,7 @@
         <v>357</v>
       </c>
       <c r="B73">
-        <v>0.4921052631578947</v>
+        <v>0.4338983050847458</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -4762,7 +4762,7 @@
         <v>358</v>
       </c>
       <c r="B74">
-        <v>0.5697211155378487</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -4770,7 +4770,7 @@
         <v>359</v>
       </c>
       <c r="B75">
-        <v>0.5942857142857143</v>
+        <v>0.5281173594132029</v>
       </c>
     </row>
   </sheetData>
@@ -4799,7 +4799,7 @@
         <v>360</v>
       </c>
       <c r="B2">
-        <v>0.3651994497936726</v>
+        <v>0.3278787878787879</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -4807,7 +4807,7 @@
         <v>361</v>
       </c>
       <c r="B3">
-        <v>0.4794007490636704</v>
+        <v>0.4364820846905538</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -4815,7 +4815,7 @@
         <v>362</v>
       </c>
       <c r="B4">
-        <v>0.4671875</v>
+        <v>0.4060052219321149</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -4823,7 +4823,7 @@
         <v>363</v>
       </c>
       <c r="B5">
-        <v>0.6052631578947368</v>
+        <v>0.5422222222222223</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -4831,7 +4831,7 @@
         <v>364</v>
       </c>
       <c r="B6">
-        <v>0.3074884029158383</v>
+        <v>0.2707744488411532</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -4839,7 +4839,7 @@
         <v>365</v>
       </c>
       <c r="B7">
-        <v>0.4149305555555556</v>
+        <v>0.3679525222551929</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -4847,7 +4847,7 @@
         <v>366</v>
       </c>
       <c r="B8">
-        <v>0.6010362694300518</v>
+        <v>0.5530973451327433</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -4855,7 +4855,7 @@
         <v>367</v>
       </c>
       <c r="B9">
-        <v>0.460559796437659</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -4863,7 +4863,7 @@
         <v>368</v>
       </c>
       <c r="B10">
-        <v>0.5252808988764045</v>
+        <v>0.4663461538461539</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -4871,7 +4871,7 @@
         <v>369</v>
       </c>
       <c r="B11">
-        <v>0.5062586926286509</v>
+        <v>0.430365296803653</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -4879,7 +4879,7 @@
         <v>370</v>
       </c>
       <c r="B12">
-        <v>0.4245283018867925</v>
+        <v>0.3775100401606425</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -4887,7 +4887,7 @@
         <v>371</v>
       </c>
       <c r="B13">
-        <v>0.4556390977443609</v>
+        <v>0.3984962406015037</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -4895,7 +4895,7 @@
         <v>372</v>
       </c>
       <c r="B14">
-        <v>0.4095634095634096</v>
+        <v>0.3642086330935252</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -4903,7 +4903,7 @@
         <v>373</v>
       </c>
       <c r="B15">
-        <v>0.5673758865248227</v>
+        <v>0.504424778761062</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -4911,7 +4911,7 @@
         <v>374</v>
       </c>
       <c r="B16">
-        <v>0.3330693069306931</v>
+        <v>0.2838240158782666</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -4919,7 +4919,7 @@
         <v>375</v>
       </c>
       <c r="B17">
-        <v>0.3605697151424288</v>
+        <v>0.3128950695322377</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -4927,7 +4927,7 @@
         <v>376</v>
       </c>
       <c r="B18">
-        <v>0.5180327868852459</v>
+        <v>0.4796511627906977</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -4935,7 +4935,7 @@
         <v>377</v>
       </c>
       <c r="B19">
-        <v>0.4071146245059288</v>
+        <v>0.3594994311717861</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -4943,7 +4943,7 @@
         <v>378</v>
       </c>
       <c r="B20">
-        <v>0.4185248713550601</v>
+        <v>0.3646723646723647</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -4951,7 +4951,7 @@
         <v>379</v>
       </c>
       <c r="B21">
-        <v>0.3853989813242784</v>
+        <v>0.3401609363569861</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -4959,7 +4959,7 @@
         <v>380</v>
       </c>
       <c r="B22">
-        <v>0.4078212290502793</v>
+        <v>0.3478927203065134</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -4967,7 +4967,7 @@
         <v>381</v>
       </c>
       <c r="B23">
-        <v>0.4715127701375246</v>
+        <v>0.4114754098360656</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -4975,7 +4975,7 @@
         <v>382</v>
       </c>
       <c r="B24">
-        <v>0.4276807980049875</v>
+        <v>0.3658536585365854</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -4983,7 +4983,7 @@
         <v>383</v>
       </c>
       <c r="B25">
-        <v>0.4417670682730924</v>
+        <v>0.3804713804713805</v>
       </c>
     </row>
     <row r="26" spans="1:2">
@@ -4991,7 +4991,7 @@
         <v>384</v>
       </c>
       <c r="B26">
-        <v>0.4021655065738592</v>
+        <v>0.3308733087330873</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -4999,7 +4999,7 @@
         <v>385</v>
       </c>
       <c r="B27">
-        <v>0.4928684627575277</v>
+        <v>0.4227748691099477</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -5007,7 +5007,7 @@
         <v>386</v>
       </c>
       <c r="B28">
-        <v>0.5111111111111111</v>
+        <v>0.4397350993377483</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -5015,7 +5015,7 @@
         <v>387</v>
       </c>
       <c r="B29">
-        <v>0.4424778761061947</v>
+        <v>0.4024767801857585</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -5023,7 +5023,7 @@
         <v>388</v>
       </c>
       <c r="B30">
-        <v>0.410062893081761</v>
+        <v>0.3661971830985916</v>
       </c>
     </row>
     <row r="31" spans="1:2">
@@ -5031,7 +5031,7 @@
         <v>389</v>
       </c>
       <c r="B31">
-        <v>0.4387211367673179</v>
+        <v>0.3891402714932127</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -5039,7 +5039,7 @@
         <v>390</v>
       </c>
       <c r="B32">
-        <v>0.3718562874251497</v>
+        <v>0.3269824922760041</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -5047,7 +5047,7 @@
         <v>391</v>
       </c>
       <c r="B33">
-        <v>0.6409090909090909</v>
+        <v>0.5404411764705882</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -5055,7 +5055,7 @@
         <v>392</v>
       </c>
       <c r="B34">
-        <v>0.4546875</v>
+        <v>0.3919793014230272</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -5063,7 +5063,7 @@
         <v>393</v>
       </c>
       <c r="B35">
-        <v>0.4166666666666667</v>
+        <v>0.3505747126436782</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -5071,7 +5071,7 @@
         <v>394</v>
       </c>
       <c r="B36">
-        <v>0.3780160857908847</v>
+        <v>0.3303370786516854</v>
       </c>
     </row>
     <row r="37" spans="1:2">
@@ -5079,7 +5079,7 @@
         <v>395</v>
       </c>
       <c r="B37">
-        <v>0.5656565656565656</v>
+        <v>0.507908611599297</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -5087,7 +5087,7 @@
         <v>396</v>
       </c>
       <c r="B38">
-        <v>0.451693851944793</v>
+        <v>0.3691860465116279</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -5095,7 +5095,7 @@
         <v>397</v>
       </c>
       <c r="B39">
-        <v>0.3484384568279241</v>
+        <v>0.3059193294918806</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -5103,7 +5103,7 @@
         <v>398</v>
       </c>
       <c r="B40">
-        <v>0.5864661654135338</v>
+        <v>0.5488215488215489</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -5111,7 +5111,7 @@
         <v>399</v>
       </c>
       <c r="B41">
-        <v>0.5126984126984127</v>
+        <v>0.4579310344827586</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -5119,7 +5119,7 @@
         <v>400</v>
       </c>
       <c r="B42">
-        <v>0.8367346938775511</v>
+        <v>0.7818181818181819</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -5127,7 +5127,7 @@
         <v>401</v>
       </c>
       <c r="B43">
-        <v>0.3498647430117223</v>
+        <v>0.3046757164404223</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -5135,7 +5135,7 @@
         <v>402</v>
       </c>
       <c r="B44">
-        <v>0.4119804400977995</v>
+        <v>0.3559670781893004</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -5143,7 +5143,7 @@
         <v>403</v>
       </c>
       <c r="B45">
-        <v>0.4898710865561695</v>
+        <v>0.4276923076923077</v>
       </c>
     </row>
     <row r="46" spans="1:2">
@@ -5151,7 +5151,7 @@
         <v>404</v>
       </c>
       <c r="B46">
-        <v>0.4382433668801464</v>
+        <v>0.3864353312302839</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -5159,7 +5159,7 @@
         <v>405</v>
       </c>
       <c r="B47">
-        <v>0.6125827814569537</v>
+        <v>0.521978021978022</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -5167,7 +5167,7 @@
         <v>406</v>
       </c>
       <c r="B48">
-        <v>0.536723163841808</v>
+        <v>0.4811320754716981</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -5175,7 +5175,7 @@
         <v>407</v>
       </c>
       <c r="B49">
-        <v>0.4464285714285715</v>
+        <v>0.3906432748538012</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -5183,7 +5183,7 @@
         <v>408</v>
       </c>
       <c r="B50">
-        <v>0.4760147601476015</v>
+        <v>0.4251592356687898</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -5191,7 +5191,7 @@
         <v>409</v>
       </c>
       <c r="B51">
-        <v>0.4147952443857332</v>
+        <v>0.3558215451577802</v>
       </c>
     </row>
     <row r="52" spans="1:2">
@@ -5199,7 +5199,7 @@
         <v>410</v>
       </c>
       <c r="B52">
-        <v>0.4637146371463715</v>
+        <v>0.3987603305785124</v>
       </c>
     </row>
     <row r="53" spans="1:2">
@@ -5207,7 +5207,7 @@
         <v>411</v>
       </c>
       <c r="B53">
-        <v>0.5359477124183006</v>
+        <v>0.4691358024691358</v>
       </c>
     </row>
     <row r="54" spans="1:2">
@@ -5215,7 +5215,7 @@
         <v>412</v>
       </c>
       <c r="B54">
-        <v>0.4675090252707581</v>
+        <v>0.4045112781954887</v>
       </c>
     </row>
     <row r="55" spans="1:2">
@@ -5223,7 +5223,7 @@
         <v>413</v>
       </c>
       <c r="B55">
-        <v>0.3130103429504627</v>
+        <v>0.2801703738760057</v>
       </c>
     </row>
     <row r="56" spans="1:2">
@@ -5231,7 +5231,7 @@
         <v>414</v>
       </c>
       <c r="B56">
-        <v>0.5654761904761905</v>
+        <v>0.472289156626506</v>
       </c>
     </row>
     <row r="57" spans="1:2">
@@ -5239,7 +5239,7 @@
         <v>415</v>
       </c>
       <c r="B57">
-        <v>0.3962441314553991</v>
+        <v>0.3515052888527258</v>
       </c>
     </row>
     <row r="58" spans="1:2">
@@ -5247,7 +5247,7 @@
         <v>416</v>
       </c>
       <c r="B58">
-        <v>0.5623762376237624</v>
+        <v>0.4790996784565916</v>
       </c>
     </row>
     <row r="59" spans="1:2">
@@ -5255,7 +5255,7 @@
         <v>417</v>
       </c>
       <c r="B59">
-        <v>0.4733944954128441</v>
+        <v>0.412037037037037</v>
       </c>
     </row>
     <row r="60" spans="1:2">
@@ -5263,7 +5263,7 @@
         <v>418</v>
       </c>
       <c r="B60">
-        <v>0.5013979496738118</v>
+        <v>0.4453441295546559</v>
       </c>
     </row>
     <row r="61" spans="1:2">
@@ -5271,7 +5271,7 @@
         <v>419</v>
       </c>
       <c r="B61">
-        <v>0.3907801418439716</v>
+        <v>0.3534912718204489</v>
       </c>
     </row>
     <row r="62" spans="1:2">
@@ -5279,7 +5279,7 @@
         <v>36</v>
       </c>
       <c r="B62">
-        <v>0.408016443987667</v>
+        <v>0.3688524590163935</v>
       </c>
     </row>
     <row r="63" spans="1:2">
@@ -5287,7 +5287,7 @@
         <v>420</v>
       </c>
       <c r="B63">
-        <v>0.523121387283237</v>
+        <v>0.4714640198511166</v>
       </c>
     </row>
     <row r="64" spans="1:2">
@@ -5295,7 +5295,7 @@
         <v>421</v>
       </c>
       <c r="B64">
-        <v>0.4791344667697063</v>
+        <v>0.4160206718346253</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -5303,7 +5303,7 @@
         <v>422</v>
       </c>
       <c r="B65">
-        <v>0.2831105710814095</v>
+        <v>0.2547568710359408</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -5311,7 +5311,7 @@
         <v>423</v>
       </c>
       <c r="B66">
-        <v>0.6304347826086957</v>
+        <v>0.5482456140350878</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -5319,7 +5319,7 @@
         <v>424</v>
       </c>
       <c r="B67">
-        <v>0.4653739612188366</v>
+        <v>0.397025171624714</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -5327,7 +5327,7 @@
         <v>425</v>
       </c>
       <c r="B68">
-        <v>0.2691228070175439</v>
+        <v>0.2277227722772277</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -5335,7 +5335,7 @@
         <v>426</v>
       </c>
       <c r="B69">
-        <v>0.4964285714285714</v>
+        <v>0.422514619883041</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -5343,7 +5343,7 @@
         <v>427</v>
       </c>
       <c r="B70">
-        <v>0.5323529411764706</v>
+        <v>0.4641975308641975</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -5351,7 +5351,7 @@
         <v>428</v>
       </c>
       <c r="B71">
-        <v>0.4336677814938685</v>
+        <v>0.3859480269489894</v>
       </c>
     </row>
     <row r="72" spans="1:2">
@@ -5359,7 +5359,7 @@
         <v>429</v>
       </c>
       <c r="B72">
-        <v>0.5121951219512195</v>
+        <v>0.4585537918871252</v>
       </c>
     </row>
     <row r="73" spans="1:2">
@@ -5367,7 +5367,7 @@
         <v>430</v>
       </c>
       <c r="B73">
-        <v>0.286034353995519</v>
+        <v>0.2414219474497682</v>
       </c>
     </row>
     <row r="74" spans="1:2">
@@ -5375,7 +5375,7 @@
         <v>431</v>
       </c>
       <c r="B74">
-        <v>0.5102564102564102</v>
+        <v>0.4539473684210527</v>
       </c>
     </row>
     <row r="75" spans="1:2">
@@ -5383,7 +5383,7 @@
         <v>432</v>
       </c>
       <c r="B75">
-        <v>0.377521613832853</v>
+        <v>0.3325153374233129</v>
       </c>
     </row>
     <row r="76" spans="1:2">
@@ -5391,7 +5391,7 @@
         <v>433</v>
       </c>
       <c r="B76">
-        <v>0.5620052770448549</v>
+        <v>0.5151515151515151</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -5399,7 +5399,7 @@
         <v>434</v>
       </c>
       <c r="B77">
-        <v>0.4511930585683297</v>
+        <v>0.4138576779026217</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -5407,7 +5407,7 @@
         <v>435</v>
       </c>
       <c r="B78">
-        <v>0.5008605851979346</v>
+        <v>0.434971098265896</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -5415,7 +5415,7 @@
         <v>436</v>
       </c>
       <c r="B79">
-        <v>0.4517453798767967</v>
+        <v>0.3824768323504634</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -5423,7 +5423,7 @@
         <v>437</v>
       </c>
       <c r="B80">
-        <v>0.4120762711864407</v>
+        <v>0.3660308810172571</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -5431,7 +5431,7 @@
         <v>438</v>
       </c>
       <c r="B81">
-        <v>0.5493230174081238</v>
+        <v>0.4724919093851133</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -5439,7 +5439,7 @@
         <v>439</v>
       </c>
       <c r="B82">
-        <v>0.5317604355716878</v>
+        <v>0.4639016897081413</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -5447,7 +5447,7 @@
         <v>440</v>
       </c>
       <c r="B83">
-        <v>0.5666666666666667</v>
+        <v>0.4888059701492538</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -5455,7 +5455,7 @@
         <v>441</v>
       </c>
       <c r="B84">
-        <v>0.50997150997151</v>
+        <v>0.4346793349168646</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -5463,7 +5463,7 @@
         <v>442</v>
       </c>
       <c r="B85">
-        <v>0.32996632996633</v>
+        <v>0.3002958579881657</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -5471,7 +5471,7 @@
         <v>443</v>
       </c>
       <c r="B86">
-        <v>0.3782542113323124</v>
+        <v>0.3328964613368283</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -5479,7 +5479,7 @@
         <v>444</v>
       </c>
       <c r="B87">
-        <v>0.231331592689295</v>
+        <v>0.2068809416025351</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -5487,7 +5487,7 @@
         <v>445</v>
       </c>
       <c r="B88">
-        <v>0.5376569037656904</v>
+        <v>0.4845173041894353</v>
       </c>
     </row>
     <row r="89" spans="1:2">
@@ -5495,7 +5495,7 @@
         <v>446</v>
       </c>
       <c r="B89">
-        <v>0.4484978540772532</v>
+        <v>0.3938271604938272</v>
       </c>
     </row>
     <row r="90" spans="1:2">
@@ -5503,7 +5503,7 @@
         <v>447</v>
       </c>
       <c r="B90">
-        <v>0.4240719910011249</v>
+        <v>0.383399209486166</v>
       </c>
     </row>
     <row r="91" spans="1:2">
@@ -5511,7 +5511,7 @@
         <v>448</v>
       </c>
       <c r="B91">
-        <v>0.5980707395498392</v>
+        <v>0.5258855585831063</v>
       </c>
     </row>
     <row r="92" spans="1:2">
@@ -5519,7 +5519,7 @@
         <v>449</v>
       </c>
       <c r="B92">
-        <v>0.5428571428571428</v>
+        <v>0.4867256637168141</v>
       </c>
     </row>
     <row r="93" spans="1:2">
@@ -5527,7 +5527,7 @@
         <v>450</v>
       </c>
       <c r="B93">
-        <v>0.4971428571428572</v>
+        <v>0.430622009569378</v>
       </c>
     </row>
     <row r="94" spans="1:2">
@@ -5535,7 +5535,7 @@
         <v>451</v>
       </c>
       <c r="B94">
-        <v>0.2553846153846154</v>
+        <v>0.2285460204535349</v>
       </c>
     </row>
     <row r="95" spans="1:2">
@@ -5543,7 +5543,7 @@
         <v>452</v>
       </c>
       <c r="B95">
-        <v>0.4159941305942773</v>
+        <v>0.357843137254902</v>
       </c>
     </row>
     <row r="96" spans="1:2">
@@ -5551,7 +5551,7 @@
         <v>453</v>
       </c>
       <c r="B96">
-        <v>0.5190258751902588</v>
+        <v>0.4553686934023286</v>
       </c>
     </row>
     <row r="97" spans="1:2">
@@ -5559,7 +5559,7 @@
         <v>454</v>
       </c>
       <c r="B97">
-        <v>0.5747800586510264</v>
+        <v>0.5037406483790524</v>
       </c>
     </row>
     <row r="98" spans="1:2">
@@ -5567,7 +5567,7 @@
         <v>455</v>
       </c>
       <c r="B98">
-        <v>0.5747800586510264</v>
+        <v>0.5037406483790524</v>
       </c>
     </row>
     <row r="99" spans="1:2">
@@ -5575,7 +5575,7 @@
         <v>456</v>
       </c>
       <c r="B99">
-        <v>0.5584415584415584</v>
+        <v>0.5082236842105263</v>
       </c>
     </row>
     <row r="100" spans="1:2">
@@ -5583,7 +5583,7 @@
         <v>457</v>
       </c>
       <c r="B100">
-        <v>0.5615141955835962</v>
+        <v>0.4641975308641975</v>
       </c>
     </row>
   </sheetData>
@@ -5612,7 +5612,7 @@
         <v>458</v>
       </c>
       <c r="B2">
-        <v>0.5260115606936416</v>
+        <v>0.4771573604060914</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -5620,7 +5620,7 @@
         <v>459</v>
       </c>
       <c r="B3">
-        <v>0.5704918032786885</v>
+        <v>0.4866310160427808</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -5628,7 +5628,7 @@
         <v>460</v>
       </c>
       <c r="B4">
-        <v>0.6115702479338843</v>
+        <v>0.5693430656934306</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -5636,7 +5636,7 @@
         <v>461</v>
       </c>
       <c r="B5">
-        <v>0.7058823529411765</v>
+        <v>0.6440677966101694</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -5644,7 +5644,7 @@
         <v>462</v>
       </c>
       <c r="B6">
-        <v>0.4724409448818898</v>
+        <v>0.4123020706455542</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -5652,7 +5652,7 @@
         <v>463</v>
       </c>
       <c r="B7">
-        <v>0.2855813953488372</v>
+        <v>0.2489100277447483</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -5660,7 +5660,7 @@
         <v>464</v>
       </c>
       <c r="B8">
-        <v>0.4509803921568628</v>
+        <v>0.3841754051477598</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -5668,7 +5668,7 @@
         <v>465</v>
       </c>
       <c r="B9">
-        <v>0.5755395683453237</v>
+        <v>0.5264797507788161</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -5676,7 +5676,7 @@
         <v>466</v>
       </c>
       <c r="B10">
-        <v>0.3461030383091149</v>
+        <v>0.3061224489795918</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -5684,7 +5684,7 @@
         <v>467</v>
       </c>
       <c r="B11">
-        <v>0.4795640326975477</v>
+        <v>0.4325581395348837</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -5692,7 +5692,7 @@
         <v>468</v>
       </c>
       <c r="B12">
-        <v>0.497164461247637</v>
+        <v>0.4475409836065574</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -5700,7 +5700,7 @@
         <v>469</v>
       </c>
       <c r="B13">
-        <v>0.5741127348643006</v>
+        <v>0.4956672443674177</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -5708,7 +5708,7 @@
         <v>470</v>
       </c>
       <c r="B14">
-        <v>0.4714064914992272</v>
+        <v>0.3841536614645858</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -5716,7 +5716,7 @@
         <v>471</v>
       </c>
       <c r="B15">
-        <v>0.5053995680345572</v>
+        <v>0.4432432432432433</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -5724,7 +5724,7 @@
         <v>472</v>
       </c>
       <c r="B16">
-        <v>0.6497175141242938</v>
+        <v>0.5668202764976958</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -5732,7 +5732,7 @@
         <v>473</v>
       </c>
       <c r="B17">
-        <v>0.348120764017252</v>
+        <v>0.299429164504411</v>
       </c>
     </row>
     <row r="18" spans="1:2">
@@ -5740,7 +5740,7 @@
         <v>474</v>
       </c>
       <c r="B18">
-        <v>0.7014925373134329</v>
+        <v>0.6538461538461539</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -5748,7 +5748,7 @@
         <v>475</v>
       </c>
       <c r="B19">
-        <v>0.4362017804154303</v>
+        <v>0.3940949935815148</v>
       </c>
     </row>
   </sheetData>
@@ -5801,25 +5801,25 @@
         <v>19</v>
       </c>
       <c r="C2">
-        <v>0.5192721041242221</v>
+        <v>0.4729571175259619</v>
       </c>
       <c r="D2">
-        <v>0.1254456062562416</v>
+        <v>0.1250703475929062</v>
       </c>
       <c r="E2">
-        <v>0.3421400264200792</v>
+        <v>0.2982273201251304</v>
       </c>
       <c r="F2">
-        <v>0.4454006907908317</v>
+        <v>0.3999976300571946</v>
       </c>
       <c r="G2">
-        <v>0.5194805194805194</v>
+        <v>0.4594594594594595</v>
       </c>
       <c r="H2">
-        <v>0.5811284353098669</v>
+        <v>0.5212848297213623</v>
       </c>
       <c r="I2">
-        <v>0.796875</v>
+        <v>0.7567567567567568</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -5830,25 +5830,25 @@
         <v>113</v>
       </c>
       <c r="C3">
-        <v>0.5182182464446381</v>
+        <v>0.4678260212132892</v>
       </c>
       <c r="D3">
-        <v>0.116926660402847</v>
+        <v>0.1152995921084801</v>
       </c>
       <c r="E3">
-        <v>0.2544209925841415</v>
+        <v>0.2157190635451505</v>
       </c>
       <c r="F3">
-        <v>0.446078431372549</v>
+        <v>0.39648033126294</v>
       </c>
       <c r="G3">
-        <v>0.5205479452054794</v>
+        <v>0.46723044397463</v>
       </c>
       <c r="H3">
-        <v>0.5982142857142857</v>
+        <v>0.5359477124183006</v>
       </c>
       <c r="I3">
-        <v>0.95</v>
+        <v>0.9565217391304348</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -5859,22 +5859,22 @@
         <v>152</v>
       </c>
       <c r="C4">
-        <v>0.5098025859971539</v>
+        <v>0.4586791781359444</v>
       </c>
       <c r="D4">
-        <v>0.1236105740163886</v>
+        <v>0.1234648368206105</v>
       </c>
       <c r="E4">
-        <v>0.215076660988075</v>
+        <v>0.1934171597633136</v>
       </c>
       <c r="F4">
-        <v>0.4310714420322629</v>
+        <v>0.3812191848460008</v>
       </c>
       <c r="G4">
-        <v>0.5011902621845261</v>
+        <v>0.4455348423676194</v>
       </c>
       <c r="H4">
-        <v>0.5682494077322445</v>
+        <v>0.5094000658385991</v>
       </c>
       <c r="I4">
         <v>1</v>
@@ -5888,25 +5888,25 @@
         <v>74</v>
       </c>
       <c r="C5">
-        <v>0.487289489846274</v>
+        <v>0.4364258214829352</v>
       </c>
       <c r="D5">
-        <v>0.138289377052996</v>
+        <v>0.1382182296809116</v>
       </c>
       <c r="E5">
-        <v>0.1692169216921692</v>
+        <v>0.1456928838951311</v>
       </c>
       <c r="F5">
-        <v>0.4176204819277108</v>
+        <v>0.3534165310900361</v>
       </c>
       <c r="G5">
-        <v>0.4721703144332096</v>
+        <v>0.4270102851799906</v>
       </c>
       <c r="H5">
-        <v>0.5691114171283205</v>
+        <v>0.5132169986594859</v>
       </c>
       <c r="I5">
-        <v>0.9285714285714286</v>
+        <v>0.8936170212765957</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -5917,25 +5917,25 @@
         <v>99</v>
       </c>
       <c r="C6">
-        <v>0.4652417538998427</v>
+        <v>0.4086198942159586</v>
       </c>
       <c r="D6">
-        <v>0.09522687798741047</v>
+        <v>0.08650220059455996</v>
       </c>
       <c r="E6">
-        <v>0.231331592689295</v>
+        <v>0.2068809416025351</v>
       </c>
       <c r="F6">
-        <v>0.4098131513225853</v>
+        <v>0.3569051077221012</v>
       </c>
       <c r="G6">
-        <v>0.4637146371463715</v>
+        <v>0.4024767801857585</v>
       </c>
       <c r="H6">
-        <v>0.5285206672240461</v>
+        <v>0.4652718423551757</v>
       </c>
       <c r="I6">
-        <v>0.8367346938775511</v>
+        <v>0.7818181818181819</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -5946,25 +5946,25 @@
         <v>18</v>
       </c>
       <c r="C7">
-        <v>0.511543399339061</v>
+        <v>0.4540301557053004</v>
       </c>
       <c r="D7">
-        <v>0.1172047286006486</v>
+        <v>0.112251685710939</v>
       </c>
       <c r="E7">
-        <v>0.2855813953488372</v>
+        <v>0.2489100277447483</v>
       </c>
       <c r="F7">
-        <v>0.4560869169924539</v>
+        <v>0.3866553022561985</v>
       </c>
       <c r="G7">
-        <v>0.5012820146410971</v>
+        <v>0.4453921134249003</v>
       </c>
       <c r="H7">
-        <v>0.5751828599750679</v>
+        <v>0.5187766241759665</v>
       </c>
       <c r="I7">
-        <v>0.7058823529411765</v>
+        <v>0.6538461538461539</v>
       </c>
     </row>
   </sheetData>

</xml_diff>